<commit_message>
update for October meeting
</commit_message>
<xml_diff>
--- a/data/project_timelines.xlsx
+++ b/data/project_timelines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/r_repositories/phd_project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ucbtds4\R_Repositories\phd_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F2F97A-5A62-6241-B0CF-C4FD6FED10C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F85D594-EC06-42BF-9618-5ECD994863E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="project_timelines" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="78">
   <si>
     <t>activity</t>
   </si>
@@ -50,9 +50,6 @@
     <t>O</t>
   </si>
   <si>
-    <t>1. Scoping review (Rodent trapping)</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -252,6 +249,12 @@
   </si>
   <si>
     <t>2.1.5. Draft manuscript (interim analysis)</t>
+  </si>
+  <si>
+    <t>1. Chapter 2 (Scoping review)</t>
+  </si>
+  <si>
+    <t>1.9. Respond to reviewer comments</t>
   </si>
 </sst>
 </file>
@@ -1096,20 +1099,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D49" activeCellId="1" sqref="B49 D49"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1123,12 +1126,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1">
         <v>44166</v>
@@ -1137,12 +1140,12 @@
         <v>44231</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>44228</v>
@@ -1151,12 +1154,12 @@
         <v>44256</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1">
         <v>44256</v>
@@ -1165,12 +1168,12 @@
         <v>44317</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1">
         <v>44317</v>
@@ -1179,12 +1182,12 @@
         <v>44378</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1">
         <v>44317</v>
@@ -1193,12 +1196,12 @@
         <v>44378</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1">
         <v>44317</v>
@@ -1207,12 +1210,12 @@
         <v>44378</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1">
         <v>44378</v>
@@ -1221,558 +1224,558 @@
         <v>44652</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1">
         <v>44652</v>
       </c>
       <c r="D9" s="1">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44855</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44870</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44075</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44147</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1">
+        <v>44166</v>
+      </c>
+      <c r="D13" s="1">
+        <v>44228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="1">
+        <v>44197</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44256</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1">
+        <v>44287</v>
+      </c>
+      <c r="D15" s="1">
+        <v>44317</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="1">
+        <v>44359</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44392</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="1">
+        <v>44378</v>
+      </c>
+      <c r="D17" s="1">
+        <v>44409</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44470</v>
+      </c>
+      <c r="D18" s="1">
+        <v>44501</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44562</v>
+      </c>
+      <c r="D19" s="1">
+        <v>44593</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1">
         <v>44652</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="1">
-        <v>44075</v>
-      </c>
-      <c r="D10" s="1">
-        <v>44197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="1">
-        <v>44147</v>
-      </c>
-      <c r="D11" s="1">
-        <v>44177</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D20" s="1">
+        <v>44682</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="1">
-        <v>44166</v>
-      </c>
-      <c r="D12" s="1">
-        <v>44228</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="1">
-        <v>44197</v>
-      </c>
-      <c r="D13" s="1">
-        <v>44256</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C21" s="1">
+        <v>44743</v>
+      </c>
+      <c r="D21" s="1">
+        <v>44774</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="1">
-        <v>44287</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1">
+        <v>44835</v>
+      </c>
+      <c r="D22" s="1">
+        <v>44866</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1">
+        <v>44927</v>
+      </c>
+      <c r="D23" s="1">
+        <v>44958</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1">
+        <v>45017</v>
+      </c>
+      <c r="D24" s="1">
+        <v>45047</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="1">
+        <v>44652</v>
+      </c>
+      <c r="D25" s="1">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="1">
         <v>44317</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="D26" s="1">
+        <v>44531</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="1">
         <v>44359</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D27" s="1">
         <v>44392</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="1">
-        <v>44378</v>
-      </c>
-      <c r="D16" s="1">
-        <v>44409</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="1">
-        <v>44470</v>
-      </c>
-      <c r="D17" s="1">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="1">
-        <v>44562</v>
-      </c>
-      <c r="D18" s="1">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="1">
+        <v>44665</v>
+      </c>
+      <c r="D28" s="1">
+        <v>44679</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="1">
+        <v>44638</v>
+      </c>
+      <c r="D29" s="1">
+        <v>44653</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="1">
         <v>44593</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="1">
+      <c r="D30" s="1">
         <v>44652</v>
       </c>
-      <c r="D19" s="1">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="1">
         <v>44682</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="1">
-        <v>44743</v>
-      </c>
-      <c r="D20" s="1">
-        <v>44774</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="1">
-        <v>44835</v>
-      </c>
-      <c r="D21" s="1">
-        <v>44866</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="1">
-        <v>44927</v>
-      </c>
-      <c r="D22" s="1">
-        <v>44958</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="1">
-        <v>45017</v>
-      </c>
-      <c r="D23" s="1">
-        <v>45047</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="1">
-        <v>44652</v>
-      </c>
-      <c r="D24" s="1">
-        <v>45078</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="1">
-        <v>44317</v>
-      </c>
-      <c r="D25" s="1">
-        <v>44531</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="1">
-        <v>44359</v>
-      </c>
-      <c r="D26" s="1">
-        <v>44392</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="1">
-        <v>44665</v>
-      </c>
-      <c r="D27" s="1">
-        <v>44679</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="1">
-        <v>44638</v>
-      </c>
-      <c r="D28" s="1">
-        <v>44653</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="D31" s="1">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" t="s">
         <v>69</v>
-      </c>
-      <c r="C29" s="1">
-        <v>44593</v>
-      </c>
-      <c r="D29" s="1">
-        <v>44652</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" s="1">
-        <v>44682</v>
-      </c>
-      <c r="D30" s="1">
-        <v>44805</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="1">
-        <v>45078</v>
-      </c>
-      <c r="D31" s="1">
-        <v>45108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" t="s">
-        <v>71</v>
       </c>
       <c r="C32" s="1">
         <v>45078</v>
       </c>
       <c r="D32" s="1">
+        <v>45108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="1">
+        <v>45078</v>
+      </c>
+      <c r="D33" s="1">
         <v>45139</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" s="1">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="1">
         <v>45139</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D34" s="1">
         <v>45170</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="1">
+        <v>44440</v>
+      </c>
+      <c r="D35" s="1">
+        <v>44531</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="1">
-        <v>44440</v>
-      </c>
-      <c r="D34" s="1">
-        <v>44531</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="C36" s="1">
+        <v>44638</v>
+      </c>
+      <c r="D36" s="1">
+        <v>44653</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="1">
+        <v>44665</v>
+      </c>
+      <c r="D37" s="1">
+        <v>44679</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="1">
-        <v>44638</v>
-      </c>
-      <c r="D35" s="1">
-        <v>44653</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="C38" s="1">
+        <v>44593</v>
+      </c>
+      <c r="D38" s="1">
+        <v>44652</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="1">
-        <v>44665</v>
-      </c>
-      <c r="D36" s="1">
-        <v>44679</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="C39" s="1">
+        <v>44774</v>
+      </c>
+      <c r="D39" s="1">
+        <v>44896</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" t="s">
         <v>53</v>
-      </c>
-      <c r="C37" s="1">
-        <v>44593</v>
-      </c>
-      <c r="D37" s="1">
-        <v>44652</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="1">
-        <v>44774</v>
-      </c>
-      <c r="D38" s="1">
-        <v>44896</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B39" t="s">
-        <v>54</v>
-      </c>
-      <c r="C39" s="1">
-        <v>45078</v>
-      </c>
-      <c r="D39" s="1">
-        <v>45108</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" t="s">
-        <v>55</v>
       </c>
       <c r="C40" s="1">
         <v>45078</v>
       </c>
       <c r="D40" s="1">
+        <v>45108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="1">
+        <v>45078</v>
+      </c>
+      <c r="D41" s="1">
         <v>45139</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>29</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="1">
+        <v>45139</v>
+      </c>
+      <c r="D42" s="1">
+        <v>45170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="1">
-        <v>45139</v>
-      </c>
-      <c r="D41" s="1">
-        <v>45170</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>11</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="C43" s="1">
+        <v>44348</v>
+      </c>
+      <c r="D43" s="1">
+        <v>44409</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" t="s">
         <v>57</v>
-      </c>
-      <c r="C42" s="1">
-        <v>44348</v>
-      </c>
-      <c r="D42" s="1">
-        <v>44409</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>11</v>
-      </c>
-      <c r="B43" t="s">
-        <v>58</v>
-      </c>
-      <c r="C43" s="1">
-        <v>44409</v>
-      </c>
-      <c r="D43" s="1">
-        <v>44440</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>11</v>
-      </c>
-      <c r="B44" t="s">
-        <v>30</v>
       </c>
       <c r="C44" s="1">
         <v>44409</v>
       </c>
       <c r="D44" s="1">
+        <v>44440</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="1">
+        <v>44409</v>
+      </c>
+      <c r="D45" s="1">
         <v>44562</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" s="1">
+        <v>44501</v>
+      </c>
+      <c r="D46" s="1">
+        <v>44593</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="1">
+        <v>44593</v>
+      </c>
+      <c r="D47" s="1">
+        <v>44621</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>11</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B48" t="s">
         <v>31</v>
-      </c>
-      <c r="C45" s="1">
-        <v>44501</v>
-      </c>
-      <c r="D45" s="1">
-        <v>44593</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>11</v>
-      </c>
-      <c r="B46" t="s">
-        <v>59</v>
-      </c>
-      <c r="C46" s="1">
-        <v>44593</v>
-      </c>
-      <c r="D46" s="1">
-        <v>44621</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>12</v>
-      </c>
-      <c r="B47" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" s="1">
-        <v>44075</v>
-      </c>
-      <c r="D47" s="1">
-        <v>44105</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>12</v>
-      </c>
-      <c r="B48" t="s">
-        <v>33</v>
       </c>
       <c r="C48" s="1">
         <v>44075</v>
@@ -1781,68 +1784,68 @@
         <v>44105</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="1">
+        <v>44075</v>
+      </c>
+      <c r="D49" s="1">
+        <v>44105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="1">
+        <v>44317</v>
+      </c>
+      <c r="D50" s="1">
+        <v>44440</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" t="s">
         <v>34</v>
       </c>
-      <c r="C49" s="1">
-        <v>44317</v>
-      </c>
-      <c r="D49" s="1">
-        <v>44440</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>12</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="C51" s="1">
+        <v>44409</v>
+      </c>
+      <c r="D51" s="1">
+        <v>44501</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" t="s">
         <v>35</v>
       </c>
-      <c r="C50" s="1">
-        <v>44409</v>
-      </c>
-      <c r="D50" s="1">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>12</v>
-      </c>
-      <c r="B51" t="s">
-        <v>36</v>
-      </c>
-      <c r="C51" s="1">
+      <c r="C52" s="1">
         <v>44713</v>
-      </c>
-      <c r="D51" s="1">
-        <v>44835</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>12</v>
-      </c>
-      <c r="B52" t="s">
-        <v>37</v>
-      </c>
-      <c r="C52" s="1">
-        <v>44774</v>
       </c>
       <c r="D52" s="1">
         <v>44835</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C53" s="1">
         <v>44774</v>
@@ -1851,227 +1854,241 @@
         <v>44835</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C54" s="1">
+        <v>44774</v>
+      </c>
+      <c r="D54" s="1">
         <v>44835</v>
       </c>
-      <c r="D54" s="1">
-        <v>45078</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="C55" s="1">
         <v>44835</v>
       </c>
       <c r="D55" s="1">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56" s="1">
+        <v>44835</v>
+      </c>
+      <c r="D56" s="1">
         <v>44866</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" s="1">
+        <v>44896</v>
+      </c>
+      <c r="D57" s="1">
+        <v>44958</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58" s="1">
+        <v>44682</v>
+      </c>
+      <c r="D58" s="1">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>12</v>
       </c>
-      <c r="B56" t="s">
-        <v>61</v>
-      </c>
-      <c r="C56" s="1">
-        <v>44896</v>
-      </c>
-      <c r="D56" s="1">
+      <c r="B59" t="s">
+        <v>39</v>
+      </c>
+      <c r="C59" s="1">
+        <v>44075</v>
+      </c>
+      <c r="D59" s="1">
+        <v>44682</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" t="s">
+        <v>40</v>
+      </c>
+      <c r="C60" s="1">
+        <v>44136</v>
+      </c>
+      <c r="D60" s="1">
+        <v>44713</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" t="s">
+        <v>41</v>
+      </c>
+      <c r="C61" s="1">
+        <v>44593</v>
+      </c>
+      <c r="D61" s="1">
+        <v>44774</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" t="s">
+        <v>42</v>
+      </c>
+      <c r="C62" s="1">
+        <v>44682</v>
+      </c>
+      <c r="D62" s="1">
+        <v>44835</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" t="s">
+        <v>43</v>
+      </c>
+      <c r="C63" s="1">
+        <v>44835</v>
+      </c>
+      <c r="D63" s="1">
         <v>44958</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>12</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B64" t="s">
         <v>62</v>
       </c>
-      <c r="C57" s="1">
-        <v>44682</v>
-      </c>
-      <c r="D57" s="1">
+      <c r="C64" s="1">
+        <v>44958</v>
+      </c>
+      <c r="D64" s="1">
+        <v>45017</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" t="s">
+        <v>63</v>
+      </c>
+      <c r="C65" s="1">
+        <v>45017</v>
+      </c>
+      <c r="D65" s="1">
         <v>45078</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>13</v>
-      </c>
-      <c r="B58" t="s">
-        <v>40</v>
-      </c>
-      <c r="C58" s="1">
-        <v>44075</v>
-      </c>
-      <c r="D58" s="1">
-        <v>44682</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>13</v>
-      </c>
-      <c r="B59" t="s">
-        <v>41</v>
-      </c>
-      <c r="C59" s="1">
-        <v>44136</v>
-      </c>
-      <c r="D59" s="1">
-        <v>44713</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>13</v>
-      </c>
-      <c r="B60" t="s">
-        <v>42</v>
-      </c>
-      <c r="C60" s="1">
-        <v>44593</v>
-      </c>
-      <c r="D60" s="1">
-        <v>44774</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>13</v>
-      </c>
-      <c r="B61" t="s">
-        <v>43</v>
-      </c>
-      <c r="C61" s="1">
-        <v>44682</v>
-      </c>
-      <c r="D61" s="1">
-        <v>44835</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>13</v>
-      </c>
-      <c r="B62" t="s">
-        <v>44</v>
-      </c>
-      <c r="C62" s="1">
-        <v>44835</v>
-      </c>
-      <c r="D62" s="1">
-        <v>44958</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>13</v>
-      </c>
-      <c r="B63" t="s">
-        <v>63</v>
-      </c>
-      <c r="C63" s="1">
-        <v>44958</v>
-      </c>
-      <c r="D63" s="1">
-        <v>45017</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>13</v>
-      </c>
-      <c r="B64" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" t="s">
         <v>64</v>
       </c>
-      <c r="C64" s="1">
-        <v>45017</v>
-      </c>
-      <c r="D64" s="1">
+      <c r="C66" s="1">
         <v>45078</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>13</v>
-      </c>
-      <c r="B65" t="s">
-        <v>65</v>
-      </c>
-      <c r="C65" s="1">
-        <v>45078</v>
-      </c>
-      <c r="D65" s="1">
+      <c r="D66" s="1">
         <v>45139</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>4</v>
-      </c>
-      <c r="B66" t="s">
-        <v>46</v>
-      </c>
-      <c r="C66" s="1">
-        <v>44075</v>
-      </c>
-      <c r="D66" s="1">
-        <v>45169</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>4</v>
       </c>
       <c r="B67" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C67" s="1">
-        <v>44440</v>
+        <v>44075</v>
       </c>
       <c r="D67" s="1">
-        <v>44470</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+        <v>45169</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>4</v>
       </c>
       <c r="B68" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C68" s="1">
-        <v>44501</v>
+        <v>44440</v>
       </c>
       <c r="D68" s="1">
-        <v>44593</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+        <v>44470</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>4</v>
       </c>
       <c r="B69" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C69" s="1">
+        <v>44501</v>
+      </c>
+      <c r="D69" s="1">
+        <v>44593</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70" t="s">
+        <v>48</v>
+      </c>
+      <c r="C70" s="1">
         <v>44927</v>
       </c>
-      <c r="D69" s="1">
+      <c r="D70" s="1">
         <v>45170</v>
       </c>
     </row>
@@ -2085,18 +2102,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2107,9 +2124,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2118,75 +2135,75 @@
         <v>45170</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1">
         <v>44231</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1">
         <v>44256</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1">
         <v>44317</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1">
         <v>44378</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1">
         <v>44378</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1">
         <v>44378</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -2195,119 +2212,119 @@
         <v>44652</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1">
         <v>44197</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1">
         <v>44177</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1">
         <v>44228</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1">
         <v>44256</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1">
         <v>44317</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="1">
         <v>44409</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1">
         <v>44501</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="1">
         <v>44593</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" s="1">
         <v>44392</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
         <v>66</v>
-      </c>
-      <c r="B19" t="s">
-        <v>67</v>
       </c>
       <c r="C19" s="1">
         <v>44392</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -2316,20 +2333,20 @@
         <v>45170</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" s="1">
         <v>44409</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
@@ -2338,42 +2355,42 @@
         <v>45170</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" s="1">
         <v>44378</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" s="1">
         <v>44105</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25" s="1">
         <v>44105</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>8</v>
@@ -2382,9 +2399,9 @@
         <v>44805</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>8</v>
@@ -2393,56 +2410,56 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28" s="1">
         <v>44470</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C29" s="1">
         <v>44593</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C30" s="1">
         <v>44440</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C31" s="1">
         <v>44562</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C32" s="1">
         <v>44440</v>

</xml_diff>